<commit_message>
still kinda broken but the values are editing correctly. there is a prioblem with the loop
</commit_message>
<xml_diff>
--- a/DummySheet2.xlsx
+++ b/DummySheet2.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>00410 / 00411</t>
+          <t xml:space="preserve">00410 </t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -516,7 +516,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>00410 / 00411</t>
+          <t xml:space="preserve">00410 </t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -541,7 +541,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>00453 / 00454</t>
+          <t xml:space="preserve">00453 </t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>00453 / 00454</t>
+          <t xml:space="preserve">00453 </t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -591,7 +591,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>00480 / 00481</t>
+          <t xml:space="preserve">00480 </t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -616,7 +616,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>00480 / 00481</t>
+          <t xml:space="preserve">00480 </t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>00733 / 00734</t>
+          <t xml:space="preserve">00733 </t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -666,7 +666,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>00733 / 00734</t>
+          <t xml:space="preserve">00733 </t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -691,7 +691,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>00744 / 00745</t>
+          <t xml:space="preserve">00744 </t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -716,7 +716,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>00744 / 00745</t>
+          <t xml:space="preserve">00744 </t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -741,7 +741,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>00801/00802</t>
+          <t>00801</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -760,7 +760,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>00801/00802</t>
+          <t>00801</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -779,7 +779,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>00810 / 00811</t>
+          <t xml:space="preserve">00810 </t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -798,7 +798,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>00810 / 00811</t>
+          <t xml:space="preserve">00810 </t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -817,7 +817,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>00834 / 00835</t>
+          <t xml:space="preserve">00834 </t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -836,7 +836,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>00834 / 00835</t>
+          <t xml:space="preserve">00834 </t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -855,7 +855,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>00841 / 00842</t>
+          <t xml:space="preserve">00841 </t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>00841 / 00842</t>
+          <t xml:space="preserve">00841 </t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -893,7 +893,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>00892 / 00893</t>
+          <t xml:space="preserve">00892 </t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -912,7 +912,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>00892 / 00893</t>
+          <t xml:space="preserve">00892 </t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -931,7 +931,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>00898/00899</t>
+          <t>00898</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -950,7 +950,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>00898/00899</t>
+          <t>00898</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -969,7 +969,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>00901 / 00902</t>
+          <t xml:space="preserve">00901 </t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>00901 / 00902</t>
+          <t xml:space="preserve">00901 </t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>00906 / 00907</t>
+          <t xml:space="preserve">00906 </t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>00906 / 00907</t>
+          <t xml:space="preserve">00906 </t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>00911 / 00912</t>
+          <t xml:space="preserve">00911 </t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1092,7 +1092,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>00911 / 00912</t>
+          <t xml:space="preserve">00911 </t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>00975 / 00976</t>
+          <t xml:space="preserve">00975 </t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>00975 / 00976</t>
+          <t xml:space="preserve">00975 </t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1173,7 +1173,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>00978 / 00979</t>
+          <t xml:space="preserve">00978 </t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>00978 / 00979</t>
+          <t xml:space="preserve">00978 </t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>00996/00997</t>
+          <t>00996</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>00996/00997</t>
+          <t>00996</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>00998/00999</t>
+          <t>00998</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>00998/00999</t>
+          <t>00998</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>01002/01003</t>
+          <t>01002</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>01002/01003</t>
+          <t>01002</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>01004/01005</t>
+          <t>01004</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>01004/01005</t>
+          <t>01004</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>01006/01007</t>
+          <t>01006</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>01006/01007</t>
+          <t>01006</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>01010/01011</t>
+          <t>01010</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>01010/01011</t>
+          <t>01010</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>01021 / 01022</t>
+          <t xml:space="preserve">01021 </t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>01021 / 01022</t>
+          <t xml:space="preserve">01021 </t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>01030 / 01031</t>
+          <t xml:space="preserve">01030 </t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>01030 / 01031</t>
+          <t xml:space="preserve">01030 </t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>01034 / 01035</t>
+          <t xml:space="preserve">01034 </t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>01034 / 01035</t>
+          <t xml:space="preserve">01034 </t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>01038 / 01039</t>
+          <t xml:space="preserve">01038 </t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1770,7 +1770,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>01038 / 01039</t>
+          <t xml:space="preserve">01038 </t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>01040/01041</t>
+          <t>01040</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>01040/01041</t>
+          <t>01040</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1853,15 +1853,15 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>01044(5)</t>
+          <t>01044</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>24329</v>
+        <v>24336</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1880,15 +1880,15 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>01044(5)</t>
+          <t>01044</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>24329</v>
+        <v>24336</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1907,15 +1907,15 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>01044/01045</t>
+          <t>01044(5)</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>24336</v>
+        <v>24329</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1934,15 +1934,15 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>01044/01045</t>
+          <t>01044(5)</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>24336</v>
+        <v>24329</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>01058/01059</t>
+          <t>01058</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>01058/01059</t>
+          <t>01058</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>01060/01061</t>
+          <t>01060</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>01060/01061</t>
+          <t>01060</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>01070/01071</t>
+          <t>01070</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>01070/01071</t>
+          <t>01070</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2139,7 +2139,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>01077/01078</t>
+          <t>01077</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>01077/01078</t>
+          <t>01077</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>01079/01080</t>
+          <t>01079</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>01079/01080</t>
+          <t>01079</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>01085/01086</t>
+          <t>01085</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>01085/01086</t>
+          <t>01085</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>01089/01090</t>
+          <t>01089</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>01089/01090</t>
+          <t>01089</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>01111/01112</t>
+          <t>01111</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>01111/01112</t>
+          <t>01111</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>01128/01129</t>
+          <t>01128</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>01128/01129</t>
+          <t>01128</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>01137/01138</t>
+          <t>01137</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -2510,7 +2510,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>01137/01138</t>
+          <t>01137</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>01151/01152</t>
+          <t>01151</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>01151/01152</t>
+          <t>01151</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>01172/01173</t>
+          <t>01172</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -2622,7 +2622,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>01172/01173</t>
+          <t>01172</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>01182/01183</t>
+          <t>01182</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>01182/01183</t>
+          <t>01182</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>01211/01212</t>
+          <t>01211</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>01211/01212</t>
+          <t>01211</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>01215/01216</t>
+          <t>01215</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>01215/01216</t>
+          <t>01215</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -2815,7 +2815,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>01220/01221</t>
+          <t>01220</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -2842,7 +2842,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>01220/01221</t>
+          <t>01220</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>01225/01226</t>
+          <t>01225</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2898,7 +2898,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>01225/01226</t>
+          <t>01225</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2927,7 +2927,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>01236/01237</t>
+          <t>01236</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>01236/01237</t>
+          <t>01236</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>01245/01246</t>
+          <t>01245</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3014,7 +3014,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>01245/01246</t>
+          <t>01245</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3043,7 +3043,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>01250/01251</t>
+          <t>01250</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -3070,7 +3070,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>01250/01251</t>
+          <t>01250</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -3097,7 +3097,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>01258/01259</t>
+          <t>01258</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -3124,7 +3124,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>01258/01259</t>
+          <t>01258</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>01260/01261</t>
+          <t>01260</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>01260/01261</t>
+          <t>01260</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>01284/01285</t>
+          <t>01284</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -3232,7 +3232,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>01284/01285</t>
+          <t>01284</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>01289/01290</t>
+          <t>01289</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>01289/01290</t>
+          <t>01289</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3317,7 +3317,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>01298/01299</t>
+          <t>01298</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -3344,7 +3344,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>01298/01299</t>
+          <t>01298</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>01312/01313</t>
+          <t>01312</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>01312/01313</t>
+          <t>01312</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -14872,7 +14872,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>424/5</t>
+          <t>424</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
@@ -14901,7 +14901,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>424/5</t>
+          <t>424</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">

</xml_diff>